<commit_message>
change top row color
</commit_message>
<xml_diff>
--- a/2020-03-08-ProjectMethodology-CA_Michael_Tanguy-Gantt-Lofthus.xlsx
+++ b/2020-03-08-ProjectMethodology-CA_Michael_Tanguy-Gantt-Lofthus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yugnat\Documents\Noroff\Project Management\CA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikki/Documents/Noroff FEU/Project Managment/CA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7225B6-8EBE-42DD-923D-C1D03104B619}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC122DF-379F-7D42-8056-354ECD9AFC14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="2460" windowWidth="31290" windowHeight="16830" xr2:uid="{5339A83E-B353-EF46-85FF-364D9925C28A}"/>
+    <workbookView xWindow="1600" yWindow="2460" windowWidth="31300" windowHeight="16840" xr2:uid="{5339A83E-B353-EF46-85FF-364D9925C28A}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="d/m/;@"/>
+    <numFmt numFmtId="164" formatCode="d/m/;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -211,7 +211,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,24 +245,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.749992370372631"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,19 +341,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -380,18 +362,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -408,6 +378,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -953,7 +929,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1252,84 +1228,84 @@
   <dimension ref="A1:AQ52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection sqref="A1:AG1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="4.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="20" width="4.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="27" width="3.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.125" style="4" customWidth="1"/>
-    <col min="30" max="36" width="4.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="42" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="20" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="27" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.1640625" style="4" customWidth="1"/>
+    <col min="30" max="36" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="42" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="3.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:43" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="23" t="s">
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="21" t="s">
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21" t="s">
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21" t="s">
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21" t="s">
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="20"/>
-      <c r="AK1" s="20"/>
-      <c r="AL1" s="20"/>
-      <c r="AM1" s="20"/>
-      <c r="AN1" s="20"/>
-      <c r="AO1" s="20"/>
-      <c r="AP1" s="20"/>
-      <c r="AQ1" s="20"/>
-    </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36"/>
+      <c r="AO1" s="36"/>
+      <c r="AP1" s="36"/>
+      <c r="AQ1" s="36"/>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1434,7 +1410,7 @@
       <c r="AP2" s="5"/>
       <c r="AQ2" s="5"/>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
       <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1533,8 +1509,8 @@
       <c r="AP3" s="4"/>
       <c r="AQ3" s="4"/>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1581,12 +1557,12 @@
       <c r="AP4" s="4"/>
       <c r="AQ4" s="4"/>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A5" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -1595,27 +1571,27 @@
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="36"/>
-      <c r="S5" s="36"/>
-      <c r="T5" s="36"/>
-      <c r="U5" s="36"/>
-      <c r="V5" s="36"/>
-      <c r="W5" s="36"/>
-      <c r="X5" s="36"/>
-      <c r="Y5" s="36"/>
-      <c r="Z5" s="36"/>
-      <c r="AA5" s="36"/>
-      <c r="AB5" s="36"/>
-      <c r="AC5" s="36"/>
-      <c r="AD5" s="36"/>
-      <c r="AE5" s="36"/>
-      <c r="AF5" s="36"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="32"/>
+      <c r="X5" s="32"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="32"/>
+      <c r="AA5" s="32"/>
+      <c r="AB5" s="32"/>
+      <c r="AC5" s="32"/>
+      <c r="AD5" s="32"/>
+      <c r="AE5" s="32"/>
+      <c r="AF5" s="32"/>
       <c r="AG5" s="2"/>
       <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
@@ -1625,8 +1601,8 @@
       <c r="AP5" s="4"/>
       <c r="AQ5" s="4"/>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="19">
@@ -1647,8 +1623,8 @@
       <c r="AP6" s="4"/>
       <c r="AQ6" s="4"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="19">
@@ -1669,8 +1645,8 @@
       <c r="AP7" s="4"/>
       <c r="AQ7" s="4"/>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="19">
@@ -1693,22 +1669,22 @@
       <c r="AP8" s="4"/>
       <c r="AQ8" s="4"/>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="23">
         <v>1</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="29"/>
+      <c r="K9" s="25"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
@@ -1739,7 +1715,7 @@
       <c r="AP9" s="4"/>
       <c r="AQ9" s="4"/>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
@@ -1753,7 +1729,7 @@
       <c r="AP10" s="4"/>
       <c r="AQ10" s="4"/>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AK11" s="4"/>
       <c r="AL11" s="4"/>
       <c r="AM11" s="4"/>
@@ -1762,42 +1738,42 @@
       <c r="AP11" s="4"/>
       <c r="AQ11" s="4"/>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A12" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="30"/>
-      <c r="V12" s="31"/>
-      <c r="W12" s="30"/>
-      <c r="X12" s="38"/>
-      <c r="Y12" s="38"/>
-      <c r="Z12" s="38"/>
-      <c r="AA12" s="38"/>
-      <c r="AB12" s="38"/>
-      <c r="AC12" s="38"/>
-      <c r="AD12" s="38"/>
-      <c r="AE12" s="38"/>
-      <c r="AF12" s="38"/>
-      <c r="AG12" s="39"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="26"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="34"/>
+      <c r="Y12" s="34"/>
+      <c r="Z12" s="34"/>
+      <c r="AA12" s="34"/>
+      <c r="AB12" s="34"/>
+      <c r="AC12" s="34"/>
+      <c r="AD12" s="34"/>
+      <c r="AE12" s="34"/>
+      <c r="AF12" s="34"/>
+      <c r="AG12" s="35"/>
       <c r="AK12" s="4"/>
       <c r="AL12" s="4"/>
       <c r="AM12" s="4"/>
@@ -1806,8 +1782,8 @@
       <c r="AP12" s="4"/>
       <c r="AQ12" s="4"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="13">
@@ -1833,8 +1809,8 @@
       <c r="AP13" s="4"/>
       <c r="AQ13" s="4"/>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="13">
@@ -1862,8 +1838,8 @@
       <c r="AP14" s="4"/>
       <c r="AQ14" s="4"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="4">
@@ -1893,8 +1869,8 @@
       <c r="AP15" s="4"/>
       <c r="AQ15" s="4"/>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="4">
@@ -1922,8 +1898,8 @@
       <c r="AP16" s="4"/>
       <c r="AQ16" s="4"/>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="4">
@@ -1953,8 +1929,8 @@
       <c r="AP17" s="4"/>
       <c r="AQ17" s="4"/>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="4">
@@ -1985,8 +1961,8 @@
       <c r="AP18" s="4"/>
       <c r="AQ18" s="4"/>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="4">
@@ -2013,31 +1989,31 @@
       <c r="AP19" s="4"/>
       <c r="AQ19" s="4"/>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="7">
         <v>5</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="32"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="32"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="28"/>
       <c r="U20" s="7"/>
       <c r="V20" s="7"/>
       <c r="W20" s="7"/>
@@ -2059,7 +2035,7 @@
       <c r="AP20" s="4"/>
       <c r="AQ20" s="4"/>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AK21" s="4"/>
       <c r="AL21" s="4"/>
       <c r="AM21" s="4"/>
@@ -2068,7 +2044,7 @@
       <c r="AP21" s="4"/>
       <c r="AQ21" s="4"/>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AK22" s="4"/>
       <c r="AL22" s="4"/>
       <c r="AM22" s="4"/>
@@ -2077,44 +2053,44 @@
       <c r="AP22" s="4"/>
       <c r="AQ22" s="4"/>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A23" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="38">
+      <c r="B23" s="34">
         <v>6</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="38"/>
-      <c r="R23" s="38"/>
-      <c r="S23" s="38"/>
-      <c r="T23" s="38"/>
-      <c r="U23" s="38"/>
-      <c r="V23" s="38"/>
-      <c r="W23" s="38"/>
-      <c r="X23" s="30"/>
-      <c r="Y23" s="30"/>
-      <c r="Z23" s="30"/>
-      <c r="AA23" s="30"/>
-      <c r="AB23" s="30"/>
-      <c r="AC23" s="30"/>
-      <c r="AD23" s="38"/>
-      <c r="AE23" s="38"/>
-      <c r="AF23" s="38"/>
-      <c r="AG23" s="39"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34"/>
+      <c r="Q23" s="34"/>
+      <c r="R23" s="34"/>
+      <c r="S23" s="34"/>
+      <c r="T23" s="34"/>
+      <c r="U23" s="34"/>
+      <c r="V23" s="34"/>
+      <c r="W23" s="34"/>
+      <c r="X23" s="26"/>
+      <c r="Y23" s="26"/>
+      <c r="Z23" s="26"/>
+      <c r="AA23" s="26"/>
+      <c r="AB23" s="26"/>
+      <c r="AC23" s="26"/>
+      <c r="AD23" s="34"/>
+      <c r="AE23" s="34"/>
+      <c r="AF23" s="34"/>
+      <c r="AG23" s="35"/>
       <c r="AK23" s="4"/>
       <c r="AL23" s="4"/>
       <c r="AM23" s="4"/>
@@ -2123,8 +2099,8 @@
       <c r="AP23" s="4"/>
       <c r="AQ23" s="4"/>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="4">
@@ -2141,8 +2117,8 @@
       <c r="AP24" s="4"/>
       <c r="AQ24" s="4"/>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="4">
@@ -2159,8 +2135,8 @@
       <c r="AP25" s="4"/>
       <c r="AQ25" s="4"/>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A26" s="21" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="4">
@@ -2176,8 +2152,8 @@
       <c r="AP26" s="4"/>
       <c r="AQ26" s="4"/>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="4">
@@ -2193,7 +2169,7 @@
       <c r="AP27" s="4"/>
       <c r="AQ27" s="4"/>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -2235,7 +2211,7 @@
       <c r="AP28" s="4"/>
       <c r="AQ28" s="4"/>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AD29" s="13"/>
       <c r="AE29" s="13"/>
       <c r="AF29" s="13"/>
@@ -2247,42 +2223,42 @@
       <c r="AP29" s="4"/>
       <c r="AQ29" s="4"/>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A30" s="37" t="s">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A30" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
-      <c r="O30" s="38"/>
-      <c r="P30" s="38"/>
-      <c r="Q30" s="38"/>
-      <c r="R30" s="38"/>
-      <c r="S30" s="38"/>
-      <c r="T30" s="38"/>
-      <c r="U30" s="38"/>
-      <c r="V30" s="38"/>
-      <c r="W30" s="38"/>
-      <c r="X30" s="38"/>
-      <c r="Y30" s="38"/>
-      <c r="Z30" s="38"/>
-      <c r="AA30" s="38"/>
-      <c r="AB30" s="38"/>
-      <c r="AC30" s="38"/>
-      <c r="AD30" s="30"/>
-      <c r="AE30" s="30"/>
-      <c r="AF30" s="30"/>
-      <c r="AG30" s="39"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="34"/>
+      <c r="O30" s="34"/>
+      <c r="P30" s="34"/>
+      <c r="Q30" s="34"/>
+      <c r="R30" s="34"/>
+      <c r="S30" s="34"/>
+      <c r="T30" s="34"/>
+      <c r="U30" s="34"/>
+      <c r="V30" s="34"/>
+      <c r="W30" s="34"/>
+      <c r="X30" s="34"/>
+      <c r="Y30" s="34"/>
+      <c r="Z30" s="34"/>
+      <c r="AA30" s="34"/>
+      <c r="AB30" s="34"/>
+      <c r="AC30" s="34"/>
+      <c r="AD30" s="26"/>
+      <c r="AE30" s="26"/>
+      <c r="AF30" s="26"/>
+      <c r="AG30" s="35"/>
       <c r="AK30" s="4"/>
       <c r="AL30" s="4"/>
       <c r="AM30" s="4"/>
@@ -2291,8 +2267,8 @@
       <c r="AP30" s="4"/>
       <c r="AQ30" s="4"/>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A31" s="21" t="s">
         <v>32</v>
       </c>
       <c r="B31" s="4">
@@ -2312,8 +2288,8 @@
       <c r="AP31" s="4"/>
       <c r="AQ31" s="4"/>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A32" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B32" s="4">
@@ -2333,7 +2309,7 @@
       <c r="AP32" s="4"/>
       <c r="AQ32" s="4"/>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -2361,12 +2337,12 @@
       <c r="Y33" s="7"/>
       <c r="Z33" s="7"/>
       <c r="AA33" s="7"/>
-      <c r="AB33" s="33"/>
-      <c r="AC33" s="33"/>
-      <c r="AD33" s="33"/>
-      <c r="AE33" s="33"/>
-      <c r="AF33" s="33"/>
-      <c r="AG33" s="34"/>
+      <c r="AB33" s="29"/>
+      <c r="AC33" s="29"/>
+      <c r="AD33" s="29"/>
+      <c r="AE33" s="29"/>
+      <c r="AF33" s="29"/>
+      <c r="AG33" s="30"/>
       <c r="AK33" s="4"/>
       <c r="AL33" s="4"/>
       <c r="AM33" s="4"/>
@@ -2375,7 +2351,7 @@
       <c r="AP33" s="4"/>
       <c r="AQ33" s="4"/>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AK34" s="4"/>
       <c r="AL34" s="4"/>
       <c r="AM34" s="4"/>
@@ -2384,7 +2360,7 @@
       <c r="AP34" s="4"/>
       <c r="AQ34" s="4"/>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
         <v>34</v>
       </c>
@@ -2396,7 +2372,7 @@
       <c r="AP35" s="4"/>
       <c r="AQ35" s="4"/>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
         <v>35</v>
       </c>
@@ -2409,7 +2385,7 @@
       <c r="AP36" s="4"/>
       <c r="AQ36" s="4"/>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>36</v>
       </c>
@@ -2421,7 +2397,7 @@
       <c r="AP37" s="4"/>
       <c r="AQ37" s="4"/>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>37</v>
       </c>
@@ -2433,7 +2409,7 @@
       <c r="AP38" s="4"/>
       <c r="AQ38" s="4"/>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
         <v>38</v>
       </c>
@@ -2445,7 +2421,7 @@
       <c r="AP39" s="4"/>
       <c r="AQ39" s="4"/>
     </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AK40" s="4"/>
       <c r="AL40" s="4"/>
       <c r="AM40" s="4"/>
@@ -2454,7 +2430,7 @@
       <c r="AP40" s="4"/>
       <c r="AQ40" s="4"/>
     </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AK41" s="4"/>
       <c r="AL41" s="4"/>
       <c r="AM41" s="4"/>
@@ -2463,7 +2439,7 @@
       <c r="AP41" s="4"/>
       <c r="AQ41" s="4"/>
     </row>
-    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AK42" s="4"/>
       <c r="AL42" s="4"/>
       <c r="AM42" s="4"/>
@@ -2472,7 +2448,7 @@
       <c r="AP42" s="4"/>
       <c r="AQ42" s="4"/>
     </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AK43" s="4"/>
       <c r="AL43" s="4"/>
       <c r="AM43" s="4"/>
@@ -2481,7 +2457,7 @@
       <c r="AP43" s="4"/>
       <c r="AQ43" s="4"/>
     </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AK44" s="4"/>
       <c r="AL44" s="4"/>
       <c r="AM44" s="4"/>
@@ -2490,7 +2466,7 @@
       <c r="AP44" s="4"/>
       <c r="AQ44" s="4"/>
     </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AK45" s="4"/>
       <c r="AL45" s="4"/>
       <c r="AM45" s="4"/>
@@ -2499,7 +2475,7 @@
       <c r="AP45" s="4"/>
       <c r="AQ45" s="4"/>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AK46" s="4"/>
       <c r="AL46" s="4"/>
       <c r="AM46" s="4"/>
@@ -2508,7 +2484,7 @@
       <c r="AP46" s="4"/>
       <c r="AQ46" s="4"/>
     </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AK47" s="4"/>
       <c r="AL47" s="4"/>
       <c r="AM47" s="4"/>
@@ -2517,7 +2493,7 @@
       <c r="AP47" s="4"/>
       <c r="AQ47" s="4"/>
     </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.2">
       <c r="AK48" s="4"/>
       <c r="AL48" s="4"/>
       <c r="AM48" s="4"/>
@@ -2526,7 +2502,7 @@
       <c r="AP48" s="4"/>
       <c r="AQ48" s="4"/>
     </row>
-    <row r="49" spans="37:43" x14ac:dyDescent="0.25">
+    <row r="49" spans="37:43" x14ac:dyDescent="0.2">
       <c r="AK49" s="4"/>
       <c r="AL49" s="4"/>
       <c r="AM49" s="4"/>
@@ -2535,7 +2511,7 @@
       <c r="AP49" s="4"/>
       <c r="AQ49" s="4"/>
     </row>
-    <row r="50" spans="37:43" x14ac:dyDescent="0.25">
+    <row r="50" spans="37:43" x14ac:dyDescent="0.2">
       <c r="AK50" s="4"/>
       <c r="AL50" s="4"/>
       <c r="AM50" s="4"/>
@@ -2544,7 +2520,7 @@
       <c r="AP50" s="4"/>
       <c r="AQ50" s="4"/>
     </row>
-    <row r="51" spans="37:43" x14ac:dyDescent="0.25">
+    <row r="51" spans="37:43" x14ac:dyDescent="0.2">
       <c r="AK51" s="4"/>
       <c r="AL51" s="4"/>
       <c r="AM51" s="4"/>
@@ -2553,7 +2529,7 @@
       <c r="AP51" s="4"/>
       <c r="AQ51" s="4"/>
     </row>
-    <row r="52" spans="37:43" x14ac:dyDescent="0.25">
+    <row r="52" spans="37:43" x14ac:dyDescent="0.2">
       <c r="AK52" s="4"/>
       <c r="AL52" s="4"/>
       <c r="AM52" s="4"/>
@@ -2564,15 +2540,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="AM1:AQ1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="N1:R1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="S1:W1"/>
     <mergeCell ref="X1:AB1"/>
     <mergeCell ref="AC1:AG1"/>
     <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="AM1:AQ1"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="N1:R1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2587,7 +2563,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
color and layout change
</commit_message>
<xml_diff>
--- a/2020-03-08-ProjectMethodology-CA_Michael_Tanguy-Gantt-Lofthus.xlsx
+++ b/2020-03-08-ProjectMethodology-CA_Michael_Tanguy-Gantt-Lofthus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikki/Documents/Noroff FEU/Project Managment/CA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A26FAB5-852D-034E-91A0-FEBE00C63F49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB43E08-E9D1-6847-B241-D52AA3F95E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="2460" windowWidth="45620" windowHeight="22400" xr2:uid="{5339A83E-B353-EF46-85FF-364D9925C28A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="64">
   <si>
     <t>Week 1</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>Start date: 09/02-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server/Hosting </t>
   </si>
 </sst>
 </file>
@@ -281,7 +284,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,19 +305,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,6 +325,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkUp">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -444,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -460,36 +457,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1334,7 +1328,7 @@
   <dimension ref="A1:AQ52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="AL39" sqref="AL39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1356,63 +1350,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35" t="s">
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35" t="s">
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35" t="s">
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35" t="s">
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="35"/>
-      <c r="AG1" s="35"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="36"/>
-      <c r="AL1" s="36"/>
-      <c r="AM1" s="36"/>
-      <c r="AN1" s="36"/>
-      <c r="AO1" s="36"/>
-      <c r="AP1" s="36"/>
-      <c r="AQ1" s="36"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1622,7 +1616,7 @@
       <c r="AQ3" s="4"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1670,11 +1664,11 @@
       <c r="AQ4" s="4"/>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -1683,27 +1677,27 @@
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="31"/>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="31"/>
-      <c r="Z5" s="31"/>
-      <c r="AA5" s="31"/>
-      <c r="AB5" s="31"/>
-      <c r="AC5" s="31"/>
-      <c r="AD5" s="31"/>
-      <c r="AE5" s="31"/>
-      <c r="AF5" s="31"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="26"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="26"/>
+      <c r="AC5" s="26"/>
+      <c r="AD5" s="26"/>
+      <c r="AE5" s="26"/>
+      <c r="AF5" s="26"/>
       <c r="AG5" s="2"/>
       <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
@@ -1714,13 +1708,13 @@
       <c r="AQ5" s="4"/>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="17">
         <v>3</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="17" t="s">
         <v>54</v>
       </c>
       <c r="D6" s="15"/>
@@ -1738,13 +1732,13 @@
       <c r="AQ6" s="4"/>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="17">
         <v>2</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="17" t="s">
         <v>43</v>
       </c>
       <c r="D7" s="12"/>
@@ -1762,13 +1756,13 @@
       <c r="AQ7" s="4"/>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="17">
         <v>2</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="17" t="s">
         <v>55</v>
       </c>
       <c r="D8" s="12"/>
@@ -1788,45 +1782,22 @@
       <c r="AQ8" s="4"/>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="17">
         <v>1</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="7"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="7"/>
-      <c r="AD9" s="7"/>
-      <c r="AE9" s="7"/>
-      <c r="AF9" s="7"/>
-      <c r="AG9" s="8"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="K9" s="16"/>
+      <c r="AG9" s="1"/>
       <c r="AK9" s="4"/>
       <c r="AL9" s="4"/>
       <c r="AM9" s="4"/>
@@ -1836,11 +1807,45 @@
       <c r="AQ9" s="4"/>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="A10" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="21">
+        <v>3</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="8"/>
       <c r="AK10" s="4"/>
       <c r="AL10" s="4"/>
       <c r="AM10" s="4"/>
@@ -1859,41 +1864,41 @@
       <c r="AQ11" s="4"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26"/>
-      <c r="U12" s="26"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="33"/>
-      <c r="Y12" s="33"/>
-      <c r="Z12" s="33"/>
-      <c r="AA12" s="33"/>
-      <c r="AB12" s="33"/>
-      <c r="AC12" s="33"/>
-      <c r="AD12" s="33"/>
-      <c r="AE12" s="33"/>
-      <c r="AF12" s="33"/>
-      <c r="AG12" s="34"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="22"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="22"/>
+      <c r="X12" s="28"/>
+      <c r="Y12" s="28"/>
+      <c r="Z12" s="28"/>
+      <c r="AA12" s="28"/>
+      <c r="AB12" s="28"/>
+      <c r="AC12" s="28"/>
+      <c r="AD12" s="28"/>
+      <c r="AE12" s="28"/>
+      <c r="AF12" s="28"/>
+      <c r="AG12" s="29"/>
       <c r="AK12" s="4"/>
       <c r="AL12" s="4"/>
       <c r="AM12" s="4"/>
@@ -1903,7 +1908,7 @@
       <c r="AQ12" s="4"/>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="13">
@@ -1932,7 +1937,7 @@
       <c r="AQ13" s="4"/>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="13">
@@ -1963,7 +1968,7 @@
       <c r="AQ14" s="4"/>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="4">
@@ -1996,7 +2001,7 @@
       <c r="AQ15" s="4"/>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="4">
@@ -2027,7 +2032,7 @@
       <c r="AQ16" s="4"/>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="4">
@@ -2044,10 +2049,10 @@
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="17"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
       <c r="V17" s="13"/>
       <c r="W17" s="13"/>
       <c r="AG17" s="1"/>
@@ -2060,7 +2065,7 @@
       <c r="AQ17" s="4"/>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="4">
@@ -2094,7 +2099,7 @@
       <c r="AQ18" s="4"/>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="4">
@@ -2111,9 +2116,9 @@
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
       <c r="AG19" s="1"/>
       <c r="AK19" s="4"/>
       <c r="AL19" s="4"/>
@@ -2124,32 +2129,32 @@
       <c r="AQ19" s="4"/>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="7">
         <v>5</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="28"/>
-      <c r="S20" s="28"/>
-      <c r="T20" s="28"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="37"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="37"/>
       <c r="U20" s="7"/>
       <c r="V20" s="7"/>
       <c r="W20" s="7"/>
@@ -2190,43 +2195,43 @@
       <c r="AQ22" s="4"/>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="33">
+      <c r="B23" s="28">
         <v>6</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33"/>
-      <c r="R23" s="33"/>
-      <c r="S23" s="33"/>
-      <c r="T23" s="33"/>
-      <c r="U23" s="33"/>
-      <c r="V23" s="33"/>
-      <c r="W23" s="33"/>
-      <c r="X23" s="26"/>
-      <c r="Y23" s="26"/>
-      <c r="Z23" s="26"/>
-      <c r="AA23" s="26"/>
-      <c r="AB23" s="26"/>
-      <c r="AC23" s="26"/>
-      <c r="AD23" s="33"/>
-      <c r="AE23" s="33"/>
-      <c r="AF23" s="33"/>
-      <c r="AG23" s="34"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="28"/>
+      <c r="Q23" s="28"/>
+      <c r="R23" s="28"/>
+      <c r="S23" s="28"/>
+      <c r="T23" s="28"/>
+      <c r="U23" s="28"/>
+      <c r="V23" s="28"/>
+      <c r="W23" s="28"/>
+      <c r="X23" s="22"/>
+      <c r="Y23" s="22"/>
+      <c r="Z23" s="22"/>
+      <c r="AA23" s="22"/>
+      <c r="AB23" s="22"/>
+      <c r="AC23" s="22"/>
+      <c r="AD23" s="28"/>
+      <c r="AE23" s="28"/>
+      <c r="AF23" s="28"/>
+      <c r="AG23" s="29"/>
       <c r="AK23" s="4"/>
       <c r="AL23" s="4"/>
       <c r="AM23" s="4"/>
@@ -2236,7 +2241,7 @@
       <c r="AQ23" s="4"/>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="4">
@@ -2257,7 +2262,7 @@
       <c r="AQ24" s="4"/>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="4">
@@ -2278,7 +2283,7 @@
       <c r="AQ25" s="4"/>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="19" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="4">
@@ -2298,7 +2303,7 @@
       <c r="AQ26" s="4"/>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="19" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="4">
@@ -2372,41 +2377,41 @@
       <c r="AQ29" s="4"/>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
-      <c r="O30" s="33"/>
-      <c r="P30" s="33"/>
-      <c r="Q30" s="33"/>
-      <c r="R30" s="33"/>
-      <c r="S30" s="33"/>
-      <c r="T30" s="33"/>
-      <c r="U30" s="33"/>
-      <c r="V30" s="33"/>
-      <c r="W30" s="33"/>
-      <c r="X30" s="33"/>
-      <c r="Y30" s="33"/>
-      <c r="Z30" s="33"/>
-      <c r="AA30" s="33"/>
-      <c r="AB30" s="33"/>
-      <c r="AC30" s="33"/>
-      <c r="AD30" s="26"/>
-      <c r="AE30" s="26"/>
-      <c r="AF30" s="26"/>
-      <c r="AG30" s="34"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="28"/>
+      <c r="R30" s="28"/>
+      <c r="S30" s="28"/>
+      <c r="T30" s="28"/>
+      <c r="U30" s="28"/>
+      <c r="V30" s="28"/>
+      <c r="W30" s="28"/>
+      <c r="X30" s="28"/>
+      <c r="Y30" s="28"/>
+      <c r="Z30" s="28"/>
+      <c r="AA30" s="28"/>
+      <c r="AB30" s="28"/>
+      <c r="AC30" s="28"/>
+      <c r="AD30" s="22"/>
+      <c r="AE30" s="22"/>
+      <c r="AF30" s="22"/>
+      <c r="AG30" s="29"/>
       <c r="AK30" s="4"/>
       <c r="AL30" s="4"/>
       <c r="AM30" s="4"/>
@@ -2416,7 +2421,7 @@
       <c r="AQ30" s="4"/>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="19" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="4">
@@ -2440,7 +2445,7 @@
       <c r="AQ31" s="4"/>
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B32" s="4">
@@ -2454,7 +2459,7 @@
       <c r="AD32" s="13"/>
       <c r="AE32" s="16"/>
       <c r="AF32" s="16"/>
-      <c r="AG32" s="38"/>
+      <c r="AG32" s="33"/>
       <c r="AK32" s="4"/>
       <c r="AL32" s="4"/>
       <c r="AM32" s="4"/>
@@ -2493,12 +2498,12 @@
       <c r="Y33" s="7"/>
       <c r="Z33" s="7"/>
       <c r="AA33" s="7"/>
-      <c r="AB33" s="29"/>
-      <c r="AC33" s="29"/>
-      <c r="AD33" s="29"/>
-      <c r="AE33" s="29"/>
-      <c r="AF33" s="29"/>
-      <c r="AG33" s="37"/>
+      <c r="AB33" s="24"/>
+      <c r="AC33" s="24"/>
+      <c r="AD33" s="24"/>
+      <c r="AE33" s="24"/>
+      <c r="AF33" s="24"/>
+      <c r="AG33" s="32"/>
       <c r="AK33" s="4"/>
       <c r="AL33" s="4"/>
       <c r="AM33" s="4"/>
@@ -2517,7 +2522,7 @@
       <c r="AQ34" s="4"/>
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A35" s="19"/>
+      <c r="A35" s="17"/>
       <c r="AK35" s="4"/>
       <c r="AL35" s="4"/>
       <c r="AM35" s="4"/>
@@ -2527,7 +2532,7 @@
       <c r="AQ35" s="4"/>
     </row>
     <row r="36" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="17" t="s">
         <v>59</v>
       </c>
       <c r="B36" s="13"/>
@@ -2540,7 +2545,7 @@
       <c r="AQ36" s="4"/>
     </row>
     <row r="37" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="17" t="s">
         <v>60</v>
       </c>
       <c r="AK37" s="4"/>
@@ -2552,7 +2557,7 @@
       <c r="AQ37" s="4"/>
     </row>
     <row r="38" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A38" s="19"/>
+      <c r="A38" s="17"/>
       <c r="AK38" s="4"/>
       <c r="AL38" s="4"/>
       <c r="AM38" s="4"/>
@@ -2562,7 +2567,7 @@
       <c r="AQ38" s="4"/>
     </row>
     <row r="39" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A39" s="19"/>
+      <c r="A39" s="17"/>
       <c r="AK39" s="4"/>
       <c r="AL39" s="4"/>
       <c r="AM39" s="4"/>
@@ -2723,68 +2728,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="34" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="35" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="35" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="35" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="35" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="35" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final change color and layout
</commit_message>
<xml_diff>
--- a/2020-03-08-ProjectMethodology-CA_Michael_Tanguy-Gantt-Lofthus.xlsx
+++ b/2020-03-08-ProjectMethodology-CA_Michael_Tanguy-Gantt-Lofthus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikki/Documents/Noroff FEU/Project Managment/CA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1569D59-290A-794F-B764-B2212441C100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14552952-C055-EB48-8D09-9AD0677DED92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="2460" windowWidth="45620" windowHeight="22400" xr2:uid="{5339A83E-B353-EF46-85FF-364D9925C28A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t>Week 1</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t xml:space="preserve">Server/Hosting </t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -278,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,7 +308,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.749992370372631"/>
+        <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,8 +330,14 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -337,15 +346,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -375,17 +375,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -406,11 +395,15 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -420,6 +413,28 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -428,6 +443,103 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
@@ -435,49 +547,71 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,8 +823,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6362700" y="1038225"/>
-          <a:ext cx="0" cy="1543050"/>
+          <a:off x="6614583" y="1036108"/>
+          <a:ext cx="0" cy="1550459"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -922,15 +1056,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>10583</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>62442</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>10583</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>13758</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -945,8 +1079,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10591800" y="2438400"/>
-          <a:ext cx="0" cy="2352675"/>
+          <a:off x="10847916" y="2496609"/>
+          <a:ext cx="0" cy="2364316"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1322,1366 +1456,1730 @@
   <dimension ref="A1:AQ52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:A37"/>
+      <selection activeCell="AG34" sqref="AG34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5" style="4" customWidth="1"/>
-    <col min="5" max="7" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="20" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="27" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.1640625" style="4" customWidth="1"/>
-    <col min="30" max="32" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5" style="1" customWidth="1"/>
+    <col min="5" max="20" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="27" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="33" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="37" max="42" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="3.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30" t="s">
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30" t="s">
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30" t="s">
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30" t="s">
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
+      <c r="AN1" s="15"/>
+      <c r="AO1" s="15"/>
+      <c r="AP1" s="15"/>
+      <c r="AQ1" s="15"/>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="6">
         <v>43870</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="6">
         <v>43871</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="6">
         <v>43872</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="6">
         <v>43873</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="6">
         <v>43874</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="2">
         <v>43906</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="2">
         <v>43907</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="2">
         <v>43908</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="2">
         <v>43909</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="2">
         <v>43910</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="2">
         <v>43913</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="2">
         <v>43914</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="2">
         <v>43915</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="Q2" s="2">
         <v>43916</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="2">
         <v>43917</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="2">
         <v>43920</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="2">
         <v>43921</v>
       </c>
-      <c r="U2" s="5">
+      <c r="U2" s="2">
         <v>43922</v>
       </c>
-      <c r="V2" s="5">
+      <c r="V2" s="2">
         <v>43923</v>
       </c>
-      <c r="W2" s="5">
+      <c r="W2" s="2">
         <v>43924</v>
       </c>
-      <c r="X2" s="5">
+      <c r="X2" s="2">
         <v>43927</v>
       </c>
-      <c r="Y2" s="5">
+      <c r="Y2" s="2">
         <v>43928</v>
       </c>
-      <c r="Z2" s="5">
+      <c r="Z2" s="2">
         <v>43929</v>
       </c>
-      <c r="AA2" s="5">
+      <c r="AA2" s="2">
         <v>43930</v>
       </c>
-      <c r="AB2" s="5">
+      <c r="AB2" s="2">
         <v>43931</v>
       </c>
-      <c r="AC2" s="5">
+      <c r="AC2" s="2">
         <v>43934</v>
       </c>
-      <c r="AD2" s="5">
+      <c r="AD2" s="2">
         <v>43935</v>
       </c>
-      <c r="AE2" s="5">
+      <c r="AE2" s="2">
         <v>43936</v>
       </c>
-      <c r="AF2" s="5">
+      <c r="AF2" s="2">
         <v>43937</v>
       </c>
-      <c r="AG2" s="5">
+      <c r="AG2" s="2">
         <v>43938</v>
       </c>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5"/>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="5"/>
-      <c r="AO2" s="5"/>
-      <c r="AP2" s="5"/>
-      <c r="AQ2" s="5"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="T3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="U3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="V3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="W3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="X3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="Y3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Z3" s="4" t="s">
+      <c r="Z3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AA3" s="4" t="s">
+      <c r="AA3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AB3" s="4" t="s">
+      <c r="AB3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AC3" s="4" t="s">
+      <c r="AC3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AD3" s="4" t="s">
+      <c r="AD3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AE3" s="4" t="s">
+      <c r="AE3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AF3" s="4" t="s">
+      <c r="AF3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AG3" s="4" t="s">
+      <c r="AG3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AK3" s="4"/>
-      <c r="AL3" s="4"/>
-      <c r="AM3" s="4"/>
-      <c r="AN3" s="4"/>
-      <c r="AO3" s="4"/>
-      <c r="AP3" s="4"/>
-      <c r="AQ3" s="4"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AQ3" s="1"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="10"/>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4"/>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="4"/>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="4"/>
-      <c r="AQ4" s="4"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="17"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AQ4" s="1"/>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
-      <c r="Z5" s="26"/>
-      <c r="AA5" s="26"/>
-      <c r="AB5" s="26"/>
-      <c r="AC5" s="26"/>
-      <c r="AD5" s="26"/>
-      <c r="AE5" s="26"/>
-      <c r="AF5" s="26"/>
-      <c r="AG5" s="2"/>
-      <c r="AK5" s="4"/>
-      <c r="AL5" s="4"/>
-      <c r="AM5" s="4"/>
-      <c r="AN5" s="4"/>
-      <c r="AO5" s="4"/>
-      <c r="AP5" s="4"/>
-      <c r="AQ5" s="4"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="19"/>
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="19"/>
+      <c r="AG5" s="19"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="AG6" s="1"/>
-      <c r="AK6" s="4"/>
-      <c r="AL6" s="4"/>
-      <c r="AM6" s="4"/>
-      <c r="AN6" s="4"/>
-      <c r="AO6" s="4"/>
-      <c r="AP6" s="4"/>
-      <c r="AQ6" s="4"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="17"/>
+      <c r="AG6" s="17"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+      <c r="AQ6" s="1"/>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="9">
         <v>2</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="AG7" s="1"/>
-      <c r="AK7" s="4"/>
-      <c r="AL7" s="4"/>
-      <c r="AM7" s="4"/>
-      <c r="AN7" s="4"/>
-      <c r="AO7" s="4"/>
-      <c r="AP7" s="4"/>
-      <c r="AQ7" s="4"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17"/>
+      <c r="AA7" s="17"/>
+      <c r="AB7" s="17"/>
+      <c r="AC7" s="17"/>
+      <c r="AD7" s="17"/>
+      <c r="AE7" s="17"/>
+      <c r="AF7" s="17"/>
+      <c r="AG7" s="17"/>
+      <c r="AK7" s="37"/>
+      <c r="AL7" s="1"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="1"/>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
+      <c r="AQ7" s="1"/>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="9">
         <v>2</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="AG8" s="1"/>
-      <c r="AK8" s="4"/>
-      <c r="AL8" s="4"/>
-      <c r="AM8" s="4"/>
-      <c r="AN8" s="4"/>
-      <c r="AO8" s="4"/>
-      <c r="AP8" s="4"/>
-      <c r="AQ8" s="4"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="17"/>
+      <c r="AE8" s="17"/>
+      <c r="AF8" s="17"/>
+      <c r="AG8" s="17"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="1"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+      <c r="AQ8" s="1"/>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="9">
         <v>1</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="K9" s="16"/>
-      <c r="AG9" s="1"/>
-      <c r="AK9" s="4"/>
-      <c r="AL9" s="4"/>
-      <c r="AM9" s="4"/>
-      <c r="AN9" s="4"/>
-      <c r="AO9" s="4"/>
-      <c r="AP9" s="4"/>
-      <c r="AQ9" s="4"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="17"/>
+      <c r="AA9" s="17"/>
+      <c r="AB9" s="17"/>
+      <c r="AC9" s="17"/>
+      <c r="AD9" s="17"/>
+      <c r="AE9" s="17"/>
+      <c r="AF9" s="17"/>
+      <c r="AG9" s="17"/>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="1"/>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AQ9" s="1"/>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="13">
         <v>3</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7"/>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="7"/>
-      <c r="AC10" s="7"/>
-      <c r="AD10" s="7"/>
-      <c r="AE10" s="7"/>
-      <c r="AF10" s="7"/>
-      <c r="AG10" s="8"/>
-      <c r="AK10" s="4"/>
-      <c r="AL10" s="4"/>
-      <c r="AM10" s="4"/>
-      <c r="AN10" s="4"/>
-      <c r="AO10" s="4"/>
-      <c r="AP10" s="4"/>
-      <c r="AQ10" s="4"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
+      <c r="AA10" s="17"/>
+      <c r="AB10" s="17"/>
+      <c r="AC10" s="17"/>
+      <c r="AD10" s="17"/>
+      <c r="AE10" s="17"/>
+      <c r="AF10" s="17"/>
+      <c r="AG10" s="17"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="1"/>
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="1"/>
+      <c r="AQ10" s="1"/>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="AK11" s="4"/>
-      <c r="AL11" s="4"/>
-      <c r="AM11" s="4"/>
-      <c r="AN11" s="4"/>
-      <c r="AO11" s="4"/>
-      <c r="AP11" s="4"/>
-      <c r="AQ11" s="4"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AQ11" s="1"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="22"/>
-      <c r="U12" s="22"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="22"/>
-      <c r="X12" s="28"/>
-      <c r="Y12" s="28"/>
-      <c r="Z12" s="28"/>
-      <c r="AA12" s="28"/>
-      <c r="AB12" s="28"/>
-      <c r="AC12" s="28"/>
-      <c r="AD12" s="28"/>
-      <c r="AE12" s="28"/>
-      <c r="AF12" s="28"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="33"/>
+      <c r="Z12" s="33"/>
+      <c r="AA12" s="33"/>
+      <c r="AB12" s="33"/>
+      <c r="AC12" s="33"/>
+      <c r="AD12" s="33"/>
+      <c r="AE12" s="33"/>
+      <c r="AF12" s="33"/>
       <c r="AG12" s="29"/>
-      <c r="AK12" s="4"/>
-      <c r="AL12" s="4"/>
-      <c r="AM12" s="4"/>
-      <c r="AN12" s="4"/>
-      <c r="AO12" s="4"/>
-      <c r="AP12" s="4"/>
-      <c r="AQ12" s="4"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1"/>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="7">
         <v>2</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="AG13" s="1"/>
-      <c r="AK13" s="4"/>
-      <c r="AL13" s="4"/>
-      <c r="AM13" s="4"/>
-      <c r="AN13" s="4"/>
-      <c r="AO13" s="4"/>
-      <c r="AP13" s="4"/>
-      <c r="AQ13" s="4"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="25"/>
+      <c r="V13" s="25"/>
+      <c r="W13" s="25"/>
+      <c r="X13" s="25"/>
+      <c r="Y13" s="25"/>
+      <c r="Z13" s="25"/>
+      <c r="AA13" s="25"/>
+      <c r="AB13" s="25"/>
+      <c r="AC13" s="25"/>
+      <c r="AD13" s="25"/>
+      <c r="AE13" s="25"/>
+      <c r="AF13" s="25"/>
+      <c r="AG13" s="25"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="1"/>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+      <c r="AQ13" s="1"/>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="7">
         <v>2</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="AG14" s="1"/>
-      <c r="AK14" s="4"/>
-      <c r="AL14" s="4"/>
-      <c r="AM14" s="4"/>
-      <c r="AN14" s="4"/>
-      <c r="AO14" s="4"/>
-      <c r="AP14" s="4"/>
-      <c r="AQ14" s="4"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="17"/>
+      <c r="AD14" s="17"/>
+      <c r="AE14" s="17"/>
+      <c r="AF14" s="17"/>
+      <c r="AG14" s="17"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="1">
         <v>4</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
-      <c r="AG15" s="1"/>
-      <c r="AK15" s="4"/>
-      <c r="AL15" s="4"/>
-      <c r="AM15" s="4"/>
-      <c r="AN15" s="4"/>
-      <c r="AO15" s="4"/>
-      <c r="AP15" s="4"/>
-      <c r="AQ15" s="4"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+      <c r="AE15" s="17"/>
+      <c r="AF15" s="17"/>
+      <c r="AG15" s="17"/>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="1">
         <v>2</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="16"/>
-      <c r="AG16" s="1"/>
-      <c r="AK16" s="4"/>
-      <c r="AL16" s="4"/>
-      <c r="AM16" s="4"/>
-      <c r="AN16" s="4"/>
-      <c r="AO16" s="4"/>
-      <c r="AP16" s="4"/>
-      <c r="AQ16" s="4"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="22"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="17"/>
+      <c r="AD16" s="17"/>
+      <c r="AE16" s="17"/>
+      <c r="AF16" s="17"/>
+      <c r="AG16" s="17"/>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="1"/>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="1">
         <v>4</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="36"/>
-      <c r="T17" s="36"/>
-      <c r="U17" s="36"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
-      <c r="AG17" s="1"/>
-      <c r="AK17" s="4"/>
-      <c r="AL17" s="4"/>
-      <c r="AM17" s="4"/>
-      <c r="AN17" s="4"/>
-      <c r="AO17" s="4"/>
-      <c r="AP17" s="4"/>
-      <c r="AQ17" s="4"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="28"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17"/>
+      <c r="Z17" s="17"/>
+      <c r="AA17" s="17"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="17"/>
+      <c r="AD17" s="17"/>
+      <c r="AE17" s="17"/>
+      <c r="AF17" s="17"/>
+      <c r="AG17" s="17"/>
+      <c r="AK17" s="1"/>
+      <c r="AL17" s="1"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="1"/>
+      <c r="AO17" s="1"/>
+      <c r="AP17" s="1"/>
+      <c r="AQ17" s="1"/>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="1">
         <v>2</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="16"/>
-      <c r="AG18" s="1"/>
-      <c r="AK18" s="4"/>
-      <c r="AL18" s="4"/>
-      <c r="AM18" s="4"/>
-      <c r="AN18" s="4"/>
-      <c r="AO18" s="4"/>
-      <c r="AP18" s="4"/>
-      <c r="AQ18" s="4"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="17"/>
+      <c r="AB18" s="17"/>
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="17"/>
+      <c r="AE18" s="17"/>
+      <c r="AF18" s="17"/>
+      <c r="AG18" s="17"/>
+      <c r="AK18" s="1"/>
+      <c r="AL18" s="1"/>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="1"/>
+      <c r="AO18" s="1"/>
+      <c r="AP18" s="1"/>
+      <c r="AQ18" s="1"/>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="1">
         <v>3</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
-      <c r="AG19" s="1"/>
-      <c r="AK19" s="4"/>
-      <c r="AL19" s="4"/>
-      <c r="AM19" s="4"/>
-      <c r="AN19" s="4"/>
-      <c r="AO19" s="4"/>
-      <c r="AP19" s="4"/>
-      <c r="AQ19" s="4"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="17"/>
+      <c r="AD19" s="17"/>
+      <c r="AE19" s="17"/>
+      <c r="AF19" s="17"/>
+      <c r="AG19" s="17"/>
+      <c r="AK19" s="1"/>
+      <c r="AL19" s="1"/>
+      <c r="AM19" s="1"/>
+      <c r="AN19" s="1"/>
+      <c r="AO19" s="1"/>
+      <c r="AP19" s="1"/>
+      <c r="AQ19" s="1"/>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="4">
         <v>5</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="37"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="7"/>
-      <c r="Y20" s="7"/>
-      <c r="Z20" s="7"/>
-      <c r="AA20" s="7"/>
-      <c r="AB20" s="7"/>
-      <c r="AC20" s="7"/>
-      <c r="AD20" s="7"/>
-      <c r="AE20" s="7"/>
-      <c r="AF20" s="7"/>
-      <c r="AG20" s="8"/>
-      <c r="AK20" s="4"/>
-      <c r="AL20" s="4"/>
-      <c r="AM20" s="4"/>
-      <c r="AN20" s="4"/>
-      <c r="AO20" s="4"/>
-      <c r="AP20" s="4"/>
-      <c r="AQ20" s="4"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+      <c r="Y20" s="17"/>
+      <c r="Z20" s="17"/>
+      <c r="AA20" s="17"/>
+      <c r="AB20" s="17"/>
+      <c r="AC20" s="17"/>
+      <c r="AD20" s="17"/>
+      <c r="AE20" s="17"/>
+      <c r="AF20" s="17"/>
+      <c r="AG20" s="17"/>
+      <c r="AK20" s="1"/>
+      <c r="AL20" s="1"/>
+      <c r="AM20" s="1"/>
+      <c r="AN20" s="1"/>
+      <c r="AO20" s="1"/>
+      <c r="AP20" s="1"/>
+      <c r="AQ20" s="1"/>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="AK21" s="4"/>
-      <c r="AL21" s="4"/>
-      <c r="AM21" s="4"/>
-      <c r="AN21" s="4"/>
-      <c r="AO21" s="4"/>
-      <c r="AP21" s="4"/>
-      <c r="AQ21" s="4"/>
+      <c r="AK21" s="1"/>
+      <c r="AL21" s="1"/>
+      <c r="AM21" s="1"/>
+      <c r="AN21" s="1"/>
+      <c r="AO21" s="1"/>
+      <c r="AP21" s="1"/>
+      <c r="AQ21" s="1"/>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="AK22" s="4"/>
-      <c r="AL22" s="4"/>
-      <c r="AM22" s="4"/>
-      <c r="AN22" s="4"/>
-      <c r="AO22" s="4"/>
-      <c r="AP22" s="4"/>
-      <c r="AQ22" s="4"/>
+      <c r="AK22" s="1"/>
+      <c r="AL22" s="1"/>
+      <c r="AM22" s="1"/>
+      <c r="AN22" s="1"/>
+      <c r="AO22" s="1"/>
+      <c r="AP22" s="1"/>
+      <c r="AQ22" s="1"/>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="28">
+      <c r="B23" s="21">
         <v>6</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="28"/>
-      <c r="R23" s="28"/>
-      <c r="S23" s="28"/>
-      <c r="T23" s="28"/>
-      <c r="U23" s="28"/>
-      <c r="V23" s="28"/>
-      <c r="W23" s="28"/>
-      <c r="X23" s="22"/>
-      <c r="Y23" s="22"/>
-      <c r="Z23" s="22"/>
-      <c r="AA23" s="22"/>
-      <c r="AB23" s="22"/>
-      <c r="AC23" s="22"/>
-      <c r="AD23" s="28"/>
-      <c r="AE23" s="28"/>
-      <c r="AF23" s="28"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="33"/>
+      <c r="Q23" s="33"/>
+      <c r="R23" s="33"/>
+      <c r="S23" s="33"/>
+      <c r="T23" s="33"/>
+      <c r="U23" s="33"/>
+      <c r="V23" s="33"/>
+      <c r="W23" s="33"/>
+      <c r="X23" s="34"/>
+      <c r="Y23" s="34"/>
+      <c r="Z23" s="34"/>
+      <c r="AA23" s="34"/>
+      <c r="AB23" s="34"/>
+      <c r="AC23" s="34"/>
+      <c r="AD23" s="33"/>
+      <c r="AE23" s="33"/>
+      <c r="AF23" s="33"/>
       <c r="AG23" s="29"/>
-      <c r="AK23" s="4"/>
-      <c r="AL23" s="4"/>
-      <c r="AM23" s="4"/>
-      <c r="AN23" s="4"/>
-      <c r="AO23" s="4"/>
-      <c r="AP23" s="4"/>
-      <c r="AQ23" s="4"/>
+      <c r="AK23" s="1"/>
+      <c r="AL23" s="1"/>
+      <c r="AM23" s="1"/>
+      <c r="AN23" s="1"/>
+      <c r="AO23" s="1"/>
+      <c r="AP23" s="1"/>
+      <c r="AQ23" s="1"/>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="X24" s="16"/>
-      <c r="Y24" s="16"/>
-      <c r="AG24" s="1"/>
-      <c r="AK24" s="4"/>
-      <c r="AL24" s="4"/>
-      <c r="AM24" s="4"/>
-      <c r="AN24" s="4"/>
-      <c r="AO24" s="4"/>
-      <c r="AP24" s="4"/>
-      <c r="AQ24" s="4"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="25"/>
+      <c r="X24" s="31"/>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="25"/>
+      <c r="AA24" s="25"/>
+      <c r="AB24" s="25"/>
+      <c r="AC24" s="25"/>
+      <c r="AD24" s="25"/>
+      <c r="AE24" s="25"/>
+      <c r="AF24" s="25"/>
+      <c r="AG24" s="25"/>
+      <c r="AK24" s="1"/>
+      <c r="AL24" s="1"/>
+      <c r="AM24" s="1"/>
+      <c r="AN24" s="1"/>
+      <c r="AO24" s="1"/>
+      <c r="AP24" s="1"/>
+      <c r="AQ24" s="1"/>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="1">
         <v>2</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Z25" s="16"/>
-      <c r="AA25" s="16"/>
-      <c r="AG25" s="1"/>
-      <c r="AK25" s="4"/>
-      <c r="AL25" s="4"/>
-      <c r="AM25" s="4"/>
-      <c r="AN25" s="4"/>
-      <c r="AO25" s="4"/>
-      <c r="AP25" s="4"/>
-      <c r="AQ25" s="4"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="17"/>
+      <c r="Y25" s="17"/>
+      <c r="Z25" s="22"/>
+      <c r="AA25" s="22"/>
+      <c r="AB25" s="17"/>
+      <c r="AC25" s="17"/>
+      <c r="AD25" s="17"/>
+      <c r="AE25" s="17"/>
+      <c r="AF25" s="17"/>
+      <c r="AG25" s="17"/>
+      <c r="AK25" s="1"/>
+      <c r="AL25" s="1"/>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="1"/>
+      <c r="AO25" s="1"/>
+      <c r="AP25" s="1"/>
+      <c r="AQ25" s="1"/>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="1">
         <v>1</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AB26" s="16"/>
-      <c r="AG26" s="1"/>
-      <c r="AK26" s="4"/>
-      <c r="AL26" s="4"/>
-      <c r="AM26" s="4"/>
-      <c r="AN26" s="4"/>
-      <c r="AO26" s="4"/>
-      <c r="AP26" s="4"/>
-      <c r="AQ26" s="4"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="17"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="17"/>
+      <c r="Y26" s="17"/>
+      <c r="Z26" s="17"/>
+      <c r="AA26" s="17"/>
+      <c r="AB26" s="22"/>
+      <c r="AC26" s="17"/>
+      <c r="AD26" s="17"/>
+      <c r="AE26" s="17"/>
+      <c r="AF26" s="17"/>
+      <c r="AG26" s="17"/>
+      <c r="AK26" s="1"/>
+      <c r="AL26" s="1"/>
+      <c r="AM26" s="1"/>
+      <c r="AN26" s="1"/>
+      <c r="AO26" s="1"/>
+      <c r="AP26" s="1"/>
+      <c r="AQ26" s="1"/>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="1">
         <v>1</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AC27" s="16"/>
-      <c r="AG27" s="1"/>
-      <c r="AK27" s="4"/>
-      <c r="AL27" s="4"/>
-      <c r="AM27" s="4"/>
-      <c r="AN27" s="4"/>
-      <c r="AO27" s="4"/>
-      <c r="AP27" s="4"/>
-      <c r="AQ27" s="4"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="17"/>
+      <c r="U27" s="17"/>
+      <c r="V27" s="17"/>
+      <c r="W27" s="17"/>
+      <c r="X27" s="17"/>
+      <c r="Y27" s="17"/>
+      <c r="Z27" s="17"/>
+      <c r="AA27" s="17"/>
+      <c r="AB27" s="17"/>
+      <c r="AC27" s="22"/>
+      <c r="AD27" s="17"/>
+      <c r="AE27" s="17"/>
+      <c r="AF27" s="17"/>
+      <c r="AG27" s="17"/>
+      <c r="AK27" s="1"/>
+      <c r="AL27" s="1"/>
+      <c r="AM27" s="1"/>
+      <c r="AN27" s="1"/>
+      <c r="AO27" s="1"/>
+      <c r="AP27" s="1"/>
+      <c r="AQ27" s="1"/>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
-      <c r="V28" s="7"/>
-      <c r="W28" s="7"/>
-      <c r="X28" s="7"/>
-      <c r="Y28" s="7"/>
-      <c r="Z28" s="7"/>
-      <c r="AA28" s="7"/>
-      <c r="AB28" s="7"/>
-      <c r="AC28" s="7"/>
-      <c r="AD28" s="7"/>
-      <c r="AE28" s="7"/>
-      <c r="AF28" s="7"/>
-      <c r="AG28" s="8"/>
-      <c r="AK28" s="4"/>
-      <c r="AL28" s="4"/>
-      <c r="AM28" s="4"/>
-      <c r="AN28" s="4"/>
-      <c r="AO28" s="4"/>
-      <c r="AP28" s="4"/>
-      <c r="AQ28" s="4"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="17"/>
+      <c r="AA28" s="17"/>
+      <c r="AB28" s="17"/>
+      <c r="AC28" s="17"/>
+      <c r="AD28" s="17"/>
+      <c r="AE28" s="17"/>
+      <c r="AF28" s="17"/>
+      <c r="AG28" s="17"/>
+      <c r="AK28" s="1"/>
+      <c r="AL28" s="1"/>
+      <c r="AM28" s="1"/>
+      <c r="AN28" s="1"/>
+      <c r="AO28" s="1"/>
+      <c r="AP28" s="1"/>
+      <c r="AQ28" s="1"/>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="AD29" s="13"/>
-      <c r="AE29" s="13"/>
-      <c r="AF29" s="13"/>
-      <c r="AK29" s="4"/>
-      <c r="AL29" s="4"/>
-      <c r="AM29" s="4"/>
-      <c r="AN29" s="4"/>
-      <c r="AO29" s="4"/>
-      <c r="AP29" s="4"/>
-      <c r="AQ29" s="4"/>
+      <c r="AD29" s="7"/>
+      <c r="AE29" s="7"/>
+      <c r="AF29" s="7"/>
+      <c r="AK29" s="1"/>
+      <c r="AL29" s="1"/>
+      <c r="AM29" s="1"/>
+      <c r="AN29" s="1"/>
+      <c r="AO29" s="1"/>
+      <c r="AP29" s="1"/>
+      <c r="AQ29" s="1"/>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
-      <c r="O30" s="28"/>
-      <c r="P30" s="28"/>
-      <c r="Q30" s="28"/>
-      <c r="R30" s="28"/>
-      <c r="S30" s="28"/>
-      <c r="T30" s="28"/>
-      <c r="U30" s="28"/>
-      <c r="V30" s="28"/>
-      <c r="W30" s="28"/>
-      <c r="X30" s="28"/>
-      <c r="Y30" s="28"/>
-      <c r="Z30" s="28"/>
-      <c r="AA30" s="28"/>
-      <c r="AB30" s="28"/>
-      <c r="AC30" s="28"/>
-      <c r="AD30" s="22"/>
-      <c r="AE30" s="22"/>
-      <c r="AF30" s="22"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="33"/>
+      <c r="O30" s="33"/>
+      <c r="P30" s="33"/>
+      <c r="Q30" s="33"/>
+      <c r="R30" s="33"/>
+      <c r="S30" s="33"/>
+      <c r="T30" s="33"/>
+      <c r="U30" s="33"/>
+      <c r="V30" s="33"/>
+      <c r="W30" s="33"/>
+      <c r="X30" s="33"/>
+      <c r="Y30" s="33"/>
+      <c r="Z30" s="33"/>
+      <c r="AA30" s="33"/>
+      <c r="AB30" s="33"/>
+      <c r="AC30" s="33"/>
+      <c r="AD30" s="34"/>
+      <c r="AE30" s="34"/>
+      <c r="AF30" s="34"/>
       <c r="AG30" s="29"/>
-      <c r="AK30" s="4"/>
-      <c r="AL30" s="4"/>
-      <c r="AM30" s="4"/>
-      <c r="AN30" s="4"/>
-      <c r="AO30" s="4"/>
-      <c r="AP30" s="4"/>
-      <c r="AQ30" s="4"/>
+      <c r="AK30" s="1"/>
+      <c r="AL30" s="1"/>
+      <c r="AM30" s="1"/>
+      <c r="AN30" s="1"/>
+      <c r="AO30" s="1"/>
+      <c r="AP30" s="1"/>
+      <c r="AQ30" s="1"/>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="1">
         <v>1</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AB31" s="13"/>
-      <c r="AC31" s="13"/>
-      <c r="AD31" s="16"/>
-      <c r="AE31" s="13"/>
-      <c r="AF31" s="13"/>
-      <c r="AG31" s="3"/>
-      <c r="AK31" s="4"/>
-      <c r="AL31" s="4"/>
-      <c r="AM31" s="4"/>
-      <c r="AN31" s="4"/>
-      <c r="AO31" s="4"/>
-      <c r="AP31" s="4"/>
-      <c r="AQ31" s="4"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="17"/>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="17"/>
+      <c r="Y31" s="17"/>
+      <c r="Z31" s="17"/>
+      <c r="AA31" s="17"/>
+      <c r="AB31" s="27"/>
+      <c r="AC31" s="27"/>
+      <c r="AD31" s="22"/>
+      <c r="AE31" s="27"/>
+      <c r="AF31" s="27"/>
+      <c r="AG31" s="27"/>
+      <c r="AK31" s="1"/>
+      <c r="AL31" s="1"/>
+      <c r="AM31" s="1"/>
+      <c r="AN31" s="1"/>
+      <c r="AO31" s="1"/>
+      <c r="AP31" s="1"/>
+      <c r="AQ31" s="1"/>
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="1">
         <v>2</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AB32" s="13"/>
-      <c r="AC32" s="13"/>
-      <c r="AD32" s="13"/>
-      <c r="AE32" s="16"/>
-      <c r="AF32" s="16"/>
-      <c r="AG32" s="33"/>
-      <c r="AK32" s="4"/>
-      <c r="AL32" s="4"/>
-      <c r="AM32" s="4"/>
-      <c r="AN32" s="4"/>
-      <c r="AO32" s="4"/>
-      <c r="AP32" s="4"/>
-      <c r="AQ32" s="4"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="17"/>
+      <c r="AA32" s="17"/>
+      <c r="AB32" s="27"/>
+      <c r="AC32" s="27"/>
+      <c r="AD32" s="27"/>
+      <c r="AE32" s="22"/>
+      <c r="AF32" s="22"/>
+      <c r="AG32" s="35"/>
+      <c r="AK32" s="1"/>
+      <c r="AL32" s="1"/>
+      <c r="AM32" s="1"/>
+      <c r="AN32" s="1"/>
+      <c r="AO32" s="1"/>
+      <c r="AP32" s="1"/>
+      <c r="AQ32" s="1"/>
     </row>
     <row r="33" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="7"/>
-      <c r="V33" s="7"/>
-      <c r="W33" s="7"/>
-      <c r="X33" s="7"/>
-      <c r="Y33" s="7"/>
-      <c r="Z33" s="7"/>
-      <c r="AA33" s="7"/>
-      <c r="AB33" s="24"/>
-      <c r="AC33" s="24"/>
-      <c r="AD33" s="24"/>
-      <c r="AE33" s="24"/>
-      <c r="AF33" s="24"/>
-      <c r="AG33" s="32"/>
-      <c r="AK33" s="4"/>
-      <c r="AL33" s="4"/>
-      <c r="AM33" s="4"/>
-      <c r="AN33" s="4"/>
-      <c r="AO33" s="4"/>
-      <c r="AP33" s="4"/>
-      <c r="AQ33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="17"/>
+      <c r="Y33" s="17"/>
+      <c r="Z33" s="17"/>
+      <c r="AA33" s="17"/>
+      <c r="AB33" s="27"/>
+      <c r="AC33" s="27"/>
+      <c r="AD33" s="27"/>
+      <c r="AE33" s="27"/>
+      <c r="AF33" s="27"/>
+      <c r="AG33" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK33" s="1"/>
+      <c r="AL33" s="1"/>
+      <c r="AM33" s="1"/>
+      <c r="AN33" s="1"/>
+      <c r="AO33" s="1"/>
+      <c r="AP33" s="1"/>
+      <c r="AQ33" s="1"/>
     </row>
     <row r="34" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="AK34" s="4"/>
-      <c r="AL34" s="4"/>
-      <c r="AM34" s="4"/>
-      <c r="AN34" s="4"/>
-      <c r="AO34" s="4"/>
-      <c r="AP34" s="4"/>
-      <c r="AQ34" s="4"/>
+      <c r="AK34" s="1"/>
+      <c r="AL34" s="1"/>
+      <c r="AM34" s="1"/>
+      <c r="AN34" s="1"/>
+      <c r="AO34" s="1"/>
+      <c r="AP34" s="1"/>
+      <c r="AQ34" s="1"/>
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A35" s="17"/>
-      <c r="AK35" s="4"/>
-      <c r="AL35" s="4"/>
-      <c r="AM35" s="4"/>
-      <c r="AN35" s="4"/>
-      <c r="AO35" s="4"/>
-      <c r="AP35" s="4"/>
-      <c r="AQ35" s="4"/>
+      <c r="A35" s="9"/>
+      <c r="AK35" s="1"/>
+      <c r="AL35" s="1"/>
+      <c r="AM35" s="1"/>
+      <c r="AN35" s="1"/>
+      <c r="AO35" s="1"/>
+      <c r="AP35" s="1"/>
+      <c r="AQ35" s="1"/>
     </row>
     <row r="36" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A36" s="17"/>
-      <c r="B36" s="13"/>
-      <c r="AK36" s="4"/>
-      <c r="AL36" s="4"/>
-      <c r="AM36" s="4"/>
-      <c r="AN36" s="4"/>
-      <c r="AO36" s="4"/>
-      <c r="AP36" s="4"/>
-      <c r="AQ36" s="4"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="7"/>
+      <c r="AK36" s="1"/>
+      <c r="AL36" s="1"/>
+      <c r="AM36" s="1"/>
+      <c r="AN36" s="1"/>
+      <c r="AO36" s="1"/>
+      <c r="AP36" s="1"/>
+      <c r="AQ36" s="1"/>
     </row>
     <row r="37" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A37" s="17"/>
-      <c r="AK37" s="4"/>
-      <c r="AL37" s="4"/>
-      <c r="AM37" s="4"/>
-      <c r="AN37" s="4"/>
-      <c r="AO37" s="4"/>
-      <c r="AP37" s="4"/>
-      <c r="AQ37" s="4"/>
+      <c r="A37" s="9"/>
+      <c r="AK37" s="1"/>
+      <c r="AL37" s="1"/>
+      <c r="AM37" s="1"/>
+      <c r="AN37" s="1"/>
+      <c r="AO37" s="1"/>
+      <c r="AP37" s="1"/>
+      <c r="AQ37" s="1"/>
     </row>
     <row r="38" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
-      <c r="AK38" s="4"/>
-      <c r="AL38" s="4"/>
-      <c r="AM38" s="4"/>
-      <c r="AN38" s="4"/>
-      <c r="AO38" s="4"/>
-      <c r="AP38" s="4"/>
-      <c r="AQ38" s="4"/>
+      <c r="A38" s="9"/>
+      <c r="AK38" s="1"/>
+      <c r="AL38" s="1"/>
+      <c r="AM38" s="1"/>
+      <c r="AN38" s="1"/>
+      <c r="AO38" s="1"/>
+      <c r="AP38" s="1"/>
+      <c r="AQ38" s="1"/>
     </row>
     <row r="39" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A39" s="17"/>
-      <c r="AK39" s="4"/>
-      <c r="AL39" s="4"/>
-      <c r="AM39" s="4"/>
-      <c r="AN39" s="4"/>
-      <c r="AO39" s="4"/>
-      <c r="AP39" s="4"/>
-      <c r="AQ39" s="4"/>
+      <c r="A39" s="9"/>
+      <c r="AK39" s="1"/>
+      <c r="AL39" s="1"/>
+      <c r="AM39" s="1"/>
+      <c r="AN39" s="1"/>
+      <c r="AO39" s="1"/>
+      <c r="AP39" s="1"/>
+      <c r="AQ39" s="1"/>
     </row>
     <row r="40" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="AK40" s="4"/>
-      <c r="AL40" s="4"/>
-      <c r="AM40" s="4"/>
-      <c r="AN40" s="4"/>
-      <c r="AO40" s="4"/>
-      <c r="AP40" s="4"/>
-      <c r="AQ40" s="4"/>
+      <c r="AK40" s="1"/>
+      <c r="AL40" s="1"/>
+      <c r="AM40" s="1"/>
+      <c r="AN40" s="1"/>
+      <c r="AO40" s="1"/>
+      <c r="AP40" s="1"/>
+      <c r="AQ40" s="1"/>
     </row>
     <row r="41" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="AK41" s="4"/>
-      <c r="AL41" s="4"/>
-      <c r="AM41" s="4"/>
-      <c r="AN41" s="4"/>
-      <c r="AO41" s="4"/>
-      <c r="AP41" s="4"/>
-      <c r="AQ41" s="4"/>
+      <c r="AK41" s="1"/>
+      <c r="AL41" s="1"/>
+      <c r="AM41" s="1"/>
+      <c r="AN41" s="1"/>
+      <c r="AO41" s="1"/>
+      <c r="AP41" s="1"/>
+      <c r="AQ41" s="1"/>
     </row>
     <row r="42" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="AK42" s="4"/>
-      <c r="AL42" s="4"/>
-      <c r="AM42" s="4"/>
-      <c r="AN42" s="4"/>
-      <c r="AO42" s="4"/>
-      <c r="AP42" s="4"/>
-      <c r="AQ42" s="4"/>
+      <c r="AK42" s="1"/>
+      <c r="AL42" s="1"/>
+      <c r="AM42" s="1"/>
+      <c r="AN42" s="1"/>
+      <c r="AO42" s="1"/>
+      <c r="AP42" s="1"/>
+      <c r="AQ42" s="1"/>
     </row>
     <row r="43" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="AK43" s="4"/>
-      <c r="AL43" s="4"/>
-      <c r="AM43" s="4"/>
-      <c r="AN43" s="4"/>
-      <c r="AO43" s="4"/>
-      <c r="AP43" s="4"/>
-      <c r="AQ43" s="4"/>
+      <c r="AK43" s="1"/>
+      <c r="AL43" s="1"/>
+      <c r="AM43" s="1"/>
+      <c r="AN43" s="1"/>
+      <c r="AO43" s="1"/>
+      <c r="AP43" s="1"/>
+      <c r="AQ43" s="1"/>
     </row>
     <row r="44" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="AK44" s="4"/>
-      <c r="AL44" s="4"/>
-      <c r="AM44" s="4"/>
-      <c r="AN44" s="4"/>
-      <c r="AO44" s="4"/>
-      <c r="AP44" s="4"/>
-      <c r="AQ44" s="4"/>
+      <c r="AK44" s="1"/>
+      <c r="AL44" s="1"/>
+      <c r="AM44" s="1"/>
+      <c r="AN44" s="1"/>
+      <c r="AO44" s="1"/>
+      <c r="AP44" s="1"/>
+      <c r="AQ44" s="1"/>
     </row>
     <row r="45" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="AK45" s="4"/>
-      <c r="AL45" s="4"/>
-      <c r="AM45" s="4"/>
-      <c r="AN45" s="4"/>
-      <c r="AO45" s="4"/>
-      <c r="AP45" s="4"/>
-      <c r="AQ45" s="4"/>
+      <c r="AK45" s="1"/>
+      <c r="AL45" s="1"/>
+      <c r="AM45" s="1"/>
+      <c r="AN45" s="1"/>
+      <c r="AO45" s="1"/>
+      <c r="AP45" s="1"/>
+      <c r="AQ45" s="1"/>
     </row>
     <row r="46" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="AK46" s="4"/>
-      <c r="AL46" s="4"/>
-      <c r="AM46" s="4"/>
-      <c r="AN46" s="4"/>
-      <c r="AO46" s="4"/>
-      <c r="AP46" s="4"/>
-      <c r="AQ46" s="4"/>
+      <c r="AK46" s="1"/>
+      <c r="AL46" s="1"/>
+      <c r="AM46" s="1"/>
+      <c r="AN46" s="1"/>
+      <c r="AO46" s="1"/>
+      <c r="AP46" s="1"/>
+      <c r="AQ46" s="1"/>
     </row>
     <row r="47" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="AK47" s="4"/>
-      <c r="AL47" s="4"/>
-      <c r="AM47" s="4"/>
-      <c r="AN47" s="4"/>
-      <c r="AO47" s="4"/>
-      <c r="AP47" s="4"/>
-      <c r="AQ47" s="4"/>
+      <c r="AK47" s="1"/>
+      <c r="AL47" s="1"/>
+      <c r="AM47" s="1"/>
+      <c r="AN47" s="1"/>
+      <c r="AO47" s="1"/>
+      <c r="AP47" s="1"/>
+      <c r="AQ47" s="1"/>
     </row>
     <row r="48" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="AK48" s="4"/>
-      <c r="AL48" s="4"/>
-      <c r="AM48" s="4"/>
-      <c r="AN48" s="4"/>
-      <c r="AO48" s="4"/>
-      <c r="AP48" s="4"/>
-      <c r="AQ48" s="4"/>
+      <c r="AK48" s="1"/>
+      <c r="AL48" s="1"/>
+      <c r="AM48" s="1"/>
+      <c r="AN48" s="1"/>
+      <c r="AO48" s="1"/>
+      <c r="AP48" s="1"/>
+      <c r="AQ48" s="1"/>
     </row>
     <row r="49" spans="37:43" x14ac:dyDescent="0.2">
-      <c r="AK49" s="4"/>
-      <c r="AL49" s="4"/>
-      <c r="AM49" s="4"/>
-      <c r="AN49" s="4"/>
-      <c r="AO49" s="4"/>
-      <c r="AP49" s="4"/>
-      <c r="AQ49" s="4"/>
+      <c r="AK49" s="1"/>
+      <c r="AL49" s="1"/>
+      <c r="AM49" s="1"/>
+      <c r="AN49" s="1"/>
+      <c r="AO49" s="1"/>
+      <c r="AP49" s="1"/>
+      <c r="AQ49" s="1"/>
     </row>
     <row r="50" spans="37:43" x14ac:dyDescent="0.2">
-      <c r="AK50" s="4"/>
-      <c r="AL50" s="4"/>
-      <c r="AM50" s="4"/>
-      <c r="AN50" s="4"/>
-      <c r="AO50" s="4"/>
-      <c r="AP50" s="4"/>
-      <c r="AQ50" s="4"/>
+      <c r="AK50" s="1"/>
+      <c r="AL50" s="1"/>
+      <c r="AM50" s="1"/>
+      <c r="AN50" s="1"/>
+      <c r="AO50" s="1"/>
+      <c r="AP50" s="1"/>
+      <c r="AQ50" s="1"/>
     </row>
     <row r="51" spans="37:43" x14ac:dyDescent="0.2">
-      <c r="AK51" s="4"/>
-      <c r="AL51" s="4"/>
-      <c r="AM51" s="4"/>
-      <c r="AN51" s="4"/>
-      <c r="AO51" s="4"/>
-      <c r="AP51" s="4"/>
-      <c r="AQ51" s="4"/>
+      <c r="AK51" s="1"/>
+      <c r="AL51" s="1"/>
+      <c r="AM51" s="1"/>
+      <c r="AN51" s="1"/>
+      <c r="AO51" s="1"/>
+      <c r="AP51" s="1"/>
+      <c r="AQ51" s="1"/>
     </row>
     <row r="52" spans="37:43" x14ac:dyDescent="0.2">
-      <c r="AK52" s="4"/>
-      <c r="AL52" s="4"/>
-      <c r="AM52" s="4"/>
-      <c r="AN52" s="4"/>
-      <c r="AO52" s="4"/>
-      <c r="AP52" s="4"/>
-      <c r="AQ52" s="4"/>
+      <c r="AK52" s="1"/>
+      <c r="AL52" s="1"/>
+      <c r="AM52" s="1"/>
+      <c r="AN52" s="1"/>
+      <c r="AO52" s="1"/>
+      <c r="AP52" s="1"/>
+      <c r="AQ52" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2718,68 +3216,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="17" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="17" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="17" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="17" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>